<commit_message>
Aenderungen nach dem Meeting mit Hrn. Rudin sind im Dokumen angepasst
</commit_message>
<xml_diff>
--- a/01 Project Management/TechnischeRisiken.xlsx
+++ b/01 Project Management/TechnischeRisiken.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Risikomanagement</t>
   </si>
@@ -94,9 +94,6 @@
     <t>PostgreSQL</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>R…</t>
   </si>
   <si>
@@ -122,12 +119,6 @@
   </si>
   <si>
     <t>Hilfe bei Stefan Keller suchen.</t>
-  </si>
-  <si>
-    <t>Apache / Tomcat</t>
-  </si>
-  <si>
-    <t>Konfiguration Web / Server Container stellt sich schwieriger dar als angenommen. Es wird viel Zeit beansprucht die Applikationen zu konfigurieren. Gewisse Erfahrung mit diesen Komponenten ist bereits vorhanden.</t>
   </si>
 </sst>
 </file>
@@ -529,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK15"/>
+  <dimension ref="A1:AMK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,8 +583,8 @@
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="3">
-        <f>SUM(F8:F14)</f>
-        <v>32</v>
+        <f>SUM(F8:F13)</f>
+        <v>27.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -633,7 +624,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5">
         <v>30</v>
@@ -642,11 +633,11 @@
         <v>0.4</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" ref="F8:F13" si="0">D8*E8</f>
+        <f t="shared" ref="F8:F12" si="0">D8*E8</f>
         <v>12</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>17</v>
@@ -685,7 +676,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5">
         <v>30</v>
@@ -698,7 +689,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -710,7 +701,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
@@ -723,79 +714,56 @@
         <v>2</v>
       </c>
       <c r="G11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="5">
-        <v>15</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0.3</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="D15" s="7">
-        <f>SUM(D8:D13)</f>
-        <v>90</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7">
-        <f>SUM(F8:F13)</f>
-        <v>32</v>
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="D14" s="7">
+        <f>SUM(D8:D12)</f>
+        <v>75</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7">
+        <f>SUM(F8:F12)</f>
+        <v>27.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>

</xml_diff>